<commit_message>
added new calibration data to excel sheet and modified sensor_reading v3.1
</commit_message>
<xml_diff>
--- a/Calibration/calibrationdata.xlsx
+++ b/Calibration/calibrationdata.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seanj\Projects\ME121\ME121-Fishtank\Calibration_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seanj\Projects\ME121\ME121-Fishtank\Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B33700-2FB2-42F7-B291-F7890C9001A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0EA28DD-EC74-407A-AFB5-675AEA30FA72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E00AFE76-D265-496A-B5B4-331452F3FCA3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E00AFE76-D265-496A-B5B4-331452F3FCA3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Raw_data" sheetId="2" r:id="rId1"/>
+    <sheet name="Raw_data_v1" sheetId="2" r:id="rId1"/>
     <sheet name="Tabulated_data" sheetId="1" r:id="rId2"/>
+    <sheet name="Raw_data_v2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>ME121 HW3 P1 tabulated data</t>
   </si>
@@ -70,6 +71,9 @@
   </si>
   <si>
     <t>Columns in wt% NaCl</t>
+  </si>
+  <si>
+    <t>DI</t>
   </si>
 </sst>
 </file>
@@ -358,6 +362,42 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Inconsolata"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Inconsolata"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -428,42 +468,6 @@
         <scheme val="none"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Inconsolata"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Inconsolata"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -478,7 +482,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{39D6D4D1-538F-430F-84BF-C3C622A2ADB4}" name="Table3" displayName="Table3" ref="A4:D149" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{39D6D4D1-538F-430F-84BF-C3C622A2ADB4}" name="Table3" displayName="Table3" ref="A4:D149" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A4:D149" xr:uid="{BCCB55DB-627F-49C9-9118-C41FE189BDF0}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -496,7 +500,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9D3FD55C-B419-4E6A-B9C2-0F4E9994498B}" name="Table4" displayName="Table4" ref="A3:E7" totalsRowShown="0" headerRowDxfId="12" dataDxfId="13" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9D3FD55C-B419-4E6A-B9C2-0F4E9994498B}" name="Table4" displayName="Table4" ref="A3:E7" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
   <autoFilter ref="A3:E7" xr:uid="{CD512478-80EE-4F9E-875F-DEA8DEADB54B}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2894,7 +2898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8E4D6BE-55F6-4DC4-9B92-38F2D9F56896}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
@@ -2931,19 +2935,19 @@
         <v>0</v>
       </c>
       <c r="B4" s="10">
-        <f>COUNT(Raw_data!A5:A149)</f>
+        <f>COUNT(Raw_data_v1!A5:A149)</f>
         <v>145</v>
       </c>
       <c r="C4" s="16">
-        <f>AVERAGE(Raw_data!A5:A149)</f>
+        <f>AVERAGE(Raw_data_v1!A5:A149)</f>
         <v>76.34482758620689</v>
       </c>
       <c r="D4" s="17">
-        <f>_xlfn.STDEV.P(Raw_data!A5:A149)</f>
+        <f>_xlfn.STDEV.P(Raw_data_v1!A5:A149)</f>
         <v>2.7776926925798326</v>
       </c>
       <c r="E4" s="10">
-        <f>MEDIAN(Raw_data!A5:A149)</f>
+        <f>MEDIAN(Raw_data_v1!A5:A149)</f>
         <v>76</v>
       </c>
     </row>
@@ -2952,19 +2956,19 @@
         <v>0.05</v>
       </c>
       <c r="B5" s="10">
-        <f>COUNT(Raw_data!B5:B149)</f>
+        <f>COUNT(Raw_data_v1!B5:B149)</f>
         <v>145</v>
       </c>
       <c r="C5" s="16">
-        <f>AVERAGE(Raw_data!B5:B149)</f>
+        <f>AVERAGE(Raw_data_v1!B5:B149)</f>
         <v>618.68965517241384</v>
       </c>
       <c r="D5" s="17">
-        <f>_xlfn.STDEV.P(Raw_data!B5:B149)</f>
+        <f>_xlfn.STDEV.P(Raw_data_v1!B5:B149)</f>
         <v>1.8883206966793831</v>
       </c>
       <c r="E5" s="10">
-        <f>MEDIAN(Raw_data!B5:B149)</f>
+        <f>MEDIAN(Raw_data_v1!B5:B149)</f>
         <v>618</v>
       </c>
     </row>
@@ -2973,19 +2977,19 @@
         <v>0.1</v>
       </c>
       <c r="B6" s="10">
-        <f>COUNT(Raw_data!C5:C149)</f>
+        <f>COUNT(Raw_data_v1!C5:C149)</f>
         <v>145</v>
       </c>
       <c r="C6" s="16">
-        <f>AVERAGE(Raw_data!C5:C149)</f>
+        <f>AVERAGE(Raw_data_v1!C5:C149)</f>
         <v>695.8</v>
       </c>
       <c r="D6" s="17">
-        <f>_xlfn.STDEV.P(Raw_data!B5:B149)</f>
+        <f>_xlfn.STDEV.P(Raw_data_v1!B5:B149)</f>
         <v>1.8883206966793831</v>
       </c>
       <c r="E6" s="10">
-        <f>MEDIAN(Raw_data!C5:C149)</f>
+        <f>MEDIAN(Raw_data_v1!C5:C149)</f>
         <v>696</v>
       </c>
     </row>
@@ -2994,19 +2998,19 @@
         <v>0.15</v>
       </c>
       <c r="B7" s="10">
-        <f>COUNT(Raw_data!D5:D149)</f>
+        <f>COUNT(Raw_data_v1!D5:D149)</f>
         <v>145</v>
       </c>
       <c r="C7" s="16">
-        <f>AVERAGE(Raw_data!D5:D149)</f>
+        <f>AVERAGE(Raw_data_v1!D5:D149)</f>
         <v>729.72413793103453</v>
       </c>
       <c r="D7" s="17">
-        <f>_xlfn.STDEV.P(Raw_data!D5:D149)</f>
+        <f>_xlfn.STDEV.P(Raw_data_v1!D5:D149)</f>
         <v>2.3414783382643622</v>
       </c>
       <c r="E7" s="10">
-        <f>MEDIAN(Raw_data!D5:D149)</f>
+        <f>MEDIAN(Raw_data_v1!D5:D149)</f>
         <v>730</v>
       </c>
     </row>
@@ -3017,4 +3021,2413 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17ED7894-C622-4240-B7DD-597EF61256A1}">
+  <dimension ref="A1:D207"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="N120" sqref="N120"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1">
+        <v>0.05</v>
+      </c>
+      <c r="C1">
+        <v>0.1</v>
+      </c>
+      <c r="D1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>81</v>
+      </c>
+      <c r="B2">
+        <v>588</v>
+      </c>
+      <c r="C2">
+        <v>677</v>
+      </c>
+      <c r="D2">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>80</v>
+      </c>
+      <c r="B3">
+        <v>584</v>
+      </c>
+      <c r="C3">
+        <v>677</v>
+      </c>
+      <c r="D3">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>83</v>
+      </c>
+      <c r="B4">
+        <v>592</v>
+      </c>
+      <c r="C4">
+        <v>677</v>
+      </c>
+      <c r="D4">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>80</v>
+      </c>
+      <c r="B5">
+        <v>592</v>
+      </c>
+      <c r="C5">
+        <v>677</v>
+      </c>
+      <c r="D5">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>80</v>
+      </c>
+      <c r="B6">
+        <v>591</v>
+      </c>
+      <c r="C6">
+        <v>676</v>
+      </c>
+      <c r="D6">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>80</v>
+      </c>
+      <c r="B7">
+        <v>591</v>
+      </c>
+      <c r="C7">
+        <v>676</v>
+      </c>
+      <c r="D7">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>79</v>
+      </c>
+      <c r="B8">
+        <v>591</v>
+      </c>
+      <c r="C8">
+        <v>676</v>
+      </c>
+      <c r="D8">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>86</v>
+      </c>
+      <c r="B9">
+        <v>592</v>
+      </c>
+      <c r="C9">
+        <v>674</v>
+      </c>
+      <c r="D9">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>79</v>
+      </c>
+      <c r="B10">
+        <v>592</v>
+      </c>
+      <c r="C10">
+        <v>676</v>
+      </c>
+      <c r="D10">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>80</v>
+      </c>
+      <c r="B11">
+        <v>592</v>
+      </c>
+      <c r="C11">
+        <v>675</v>
+      </c>
+      <c r="D11">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>80</v>
+      </c>
+      <c r="B12">
+        <v>592</v>
+      </c>
+      <c r="C12">
+        <v>674</v>
+      </c>
+      <c r="D12">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>80</v>
+      </c>
+      <c r="B13">
+        <v>591</v>
+      </c>
+      <c r="C13">
+        <v>675</v>
+      </c>
+      <c r="D13">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>83</v>
+      </c>
+      <c r="B14">
+        <v>592</v>
+      </c>
+      <c r="C14">
+        <v>674</v>
+      </c>
+      <c r="D14">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>79</v>
+      </c>
+      <c r="B15">
+        <v>592</v>
+      </c>
+      <c r="C15">
+        <v>675</v>
+      </c>
+      <c r="D15">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>80</v>
+      </c>
+      <c r="B16">
+        <v>593</v>
+      </c>
+      <c r="C16">
+        <v>669</v>
+      </c>
+      <c r="D16">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>80</v>
+      </c>
+      <c r="B17">
+        <v>593</v>
+      </c>
+      <c r="C17">
+        <v>675</v>
+      </c>
+      <c r="D17">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>80</v>
+      </c>
+      <c r="B18">
+        <v>592</v>
+      </c>
+      <c r="C18">
+        <v>675</v>
+      </c>
+      <c r="D18">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>80</v>
+      </c>
+      <c r="B19">
+        <v>592</v>
+      </c>
+      <c r="C19">
+        <v>674</v>
+      </c>
+      <c r="D19">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>80</v>
+      </c>
+      <c r="B20">
+        <v>592</v>
+      </c>
+      <c r="C20">
+        <v>673</v>
+      </c>
+      <c r="D20">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>82</v>
+      </c>
+      <c r="B21">
+        <v>592</v>
+      </c>
+      <c r="C21">
+        <v>674</v>
+      </c>
+      <c r="D21">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>83</v>
+      </c>
+      <c r="B22">
+        <v>591</v>
+      </c>
+      <c r="C22">
+        <v>675</v>
+      </c>
+      <c r="D22">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>80</v>
+      </c>
+      <c r="B23">
+        <v>591</v>
+      </c>
+      <c r="C23">
+        <v>676</v>
+      </c>
+      <c r="D23">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>80</v>
+      </c>
+      <c r="B24">
+        <v>591</v>
+      </c>
+      <c r="C24">
+        <v>674</v>
+      </c>
+      <c r="D24">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>80</v>
+      </c>
+      <c r="B25">
+        <v>592</v>
+      </c>
+      <c r="C25">
+        <v>675</v>
+      </c>
+      <c r="D25">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>80</v>
+      </c>
+      <c r="B26">
+        <v>592</v>
+      </c>
+      <c r="C26">
+        <v>669</v>
+      </c>
+      <c r="D26">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>80</v>
+      </c>
+      <c r="B27">
+        <v>592</v>
+      </c>
+      <c r="C27">
+        <v>674</v>
+      </c>
+      <c r="D27">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>80</v>
+      </c>
+      <c r="B28">
+        <v>591</v>
+      </c>
+      <c r="C28">
+        <v>675</v>
+      </c>
+      <c r="D28">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>80</v>
+      </c>
+      <c r="B29">
+        <v>592</v>
+      </c>
+      <c r="C29">
+        <v>675</v>
+      </c>
+      <c r="D29">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>79</v>
+      </c>
+      <c r="B30">
+        <v>592</v>
+      </c>
+      <c r="C30">
+        <v>676</v>
+      </c>
+      <c r="D30">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>80</v>
+      </c>
+      <c r="B31">
+        <v>592</v>
+      </c>
+      <c r="C31">
+        <v>675</v>
+      </c>
+      <c r="D31">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>80</v>
+      </c>
+      <c r="B32">
+        <v>589</v>
+      </c>
+      <c r="C32">
+        <v>670</v>
+      </c>
+      <c r="D32">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>92</v>
+      </c>
+      <c r="B33">
+        <v>592</v>
+      </c>
+      <c r="C33">
+        <v>676</v>
+      </c>
+      <c r="D33">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>80</v>
+      </c>
+      <c r="B34">
+        <v>592</v>
+      </c>
+      <c r="C34">
+        <v>675</v>
+      </c>
+      <c r="D34">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>80</v>
+      </c>
+      <c r="B35">
+        <v>592</v>
+      </c>
+      <c r="C35">
+        <v>676</v>
+      </c>
+      <c r="D35">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>80</v>
+      </c>
+      <c r="B36">
+        <v>592</v>
+      </c>
+      <c r="C36">
+        <v>675</v>
+      </c>
+      <c r="D36">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>80</v>
+      </c>
+      <c r="B37">
+        <v>592</v>
+      </c>
+      <c r="C37">
+        <v>676</v>
+      </c>
+      <c r="D37">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>80</v>
+      </c>
+      <c r="B38">
+        <v>592</v>
+      </c>
+      <c r="C38">
+        <v>676</v>
+      </c>
+      <c r="D38">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>80</v>
+      </c>
+      <c r="B39">
+        <v>593</v>
+      </c>
+      <c r="C39">
+        <v>675</v>
+      </c>
+      <c r="D39">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>80</v>
+      </c>
+      <c r="B40">
+        <v>593</v>
+      </c>
+      <c r="C40">
+        <v>675</v>
+      </c>
+      <c r="D40">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>80</v>
+      </c>
+      <c r="B41">
+        <v>592</v>
+      </c>
+      <c r="C41">
+        <v>676</v>
+      </c>
+      <c r="D41">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>80</v>
+      </c>
+      <c r="B42">
+        <v>593</v>
+      </c>
+      <c r="C42">
+        <v>676</v>
+      </c>
+      <c r="D42">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>81</v>
+      </c>
+      <c r="B43">
+        <v>594</v>
+      </c>
+      <c r="C43">
+        <v>669</v>
+      </c>
+      <c r="D43">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>80</v>
+      </c>
+      <c r="B44">
+        <v>594</v>
+      </c>
+      <c r="C44">
+        <v>675</v>
+      </c>
+      <c r="D44">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>80</v>
+      </c>
+      <c r="B45">
+        <v>594</v>
+      </c>
+      <c r="C45">
+        <v>676</v>
+      </c>
+      <c r="D45">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>80</v>
+      </c>
+      <c r="B46">
+        <v>593</v>
+      </c>
+      <c r="C46">
+        <v>675</v>
+      </c>
+      <c r="D46">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>80</v>
+      </c>
+      <c r="B47">
+        <v>589</v>
+      </c>
+      <c r="C47">
+        <v>675</v>
+      </c>
+      <c r="D47">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>80</v>
+      </c>
+      <c r="B48">
+        <v>594</v>
+      </c>
+      <c r="C48">
+        <v>674</v>
+      </c>
+      <c r="D48">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>80</v>
+      </c>
+      <c r="B49">
+        <v>594</v>
+      </c>
+      <c r="C49">
+        <v>674</v>
+      </c>
+      <c r="D49">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>80</v>
+      </c>
+      <c r="B50">
+        <v>594</v>
+      </c>
+      <c r="C50">
+        <v>676</v>
+      </c>
+      <c r="D50">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>80</v>
+      </c>
+      <c r="B51">
+        <v>589</v>
+      </c>
+      <c r="C51">
+        <v>676</v>
+      </c>
+      <c r="D51">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>86</v>
+      </c>
+      <c r="B52">
+        <v>593</v>
+      </c>
+      <c r="C52">
+        <v>676</v>
+      </c>
+      <c r="D52">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>80</v>
+      </c>
+      <c r="B53">
+        <v>593</v>
+      </c>
+      <c r="C53">
+        <v>677</v>
+      </c>
+      <c r="D53">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>83</v>
+      </c>
+      <c r="B54">
+        <v>594</v>
+      </c>
+      <c r="C54">
+        <v>676</v>
+      </c>
+      <c r="D54">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>80</v>
+      </c>
+      <c r="B55">
+        <v>594</v>
+      </c>
+      <c r="C55">
+        <v>677</v>
+      </c>
+      <c r="D55">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>82</v>
+      </c>
+      <c r="B56">
+        <v>594</v>
+      </c>
+      <c r="C56">
+        <v>676</v>
+      </c>
+      <c r="D56">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>81</v>
+      </c>
+      <c r="B57">
+        <v>593</v>
+      </c>
+      <c r="C57">
+        <v>677</v>
+      </c>
+      <c r="D57">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>80</v>
+      </c>
+      <c r="B58">
+        <v>593</v>
+      </c>
+      <c r="C58">
+        <v>677</v>
+      </c>
+      <c r="D58">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>80</v>
+      </c>
+      <c r="B59">
+        <v>594</v>
+      </c>
+      <c r="C59">
+        <v>676</v>
+      </c>
+      <c r="D59">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>80</v>
+      </c>
+      <c r="B60">
+        <v>590</v>
+      </c>
+      <c r="C60">
+        <v>677</v>
+      </c>
+      <c r="D60">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>80</v>
+      </c>
+      <c r="B61">
+        <v>593</v>
+      </c>
+      <c r="C61">
+        <v>676</v>
+      </c>
+      <c r="D61">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>87</v>
+      </c>
+      <c r="B62">
+        <v>594</v>
+      </c>
+      <c r="C62">
+        <v>678</v>
+      </c>
+      <c r="D62">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>81</v>
+      </c>
+      <c r="B63">
+        <v>593</v>
+      </c>
+      <c r="C63">
+        <v>679</v>
+      </c>
+      <c r="D63">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>80</v>
+      </c>
+      <c r="B64">
+        <v>593</v>
+      </c>
+      <c r="C64">
+        <v>677</v>
+      </c>
+      <c r="D64">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>80</v>
+      </c>
+      <c r="B65">
+        <v>594</v>
+      </c>
+      <c r="C65">
+        <v>678</v>
+      </c>
+      <c r="D65">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>81</v>
+      </c>
+      <c r="B66">
+        <v>594</v>
+      </c>
+      <c r="C66">
+        <v>673</v>
+      </c>
+      <c r="D66">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>79</v>
+      </c>
+      <c r="B67">
+        <v>593</v>
+      </c>
+      <c r="C67">
+        <v>677</v>
+      </c>
+      <c r="D67">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>81</v>
+      </c>
+      <c r="B68">
+        <v>593</v>
+      </c>
+      <c r="C68">
+        <v>678</v>
+      </c>
+      <c r="D68">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>80</v>
+      </c>
+      <c r="B69">
+        <v>593</v>
+      </c>
+      <c r="C69">
+        <v>678</v>
+      </c>
+      <c r="D69">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>79</v>
+      </c>
+      <c r="B70">
+        <v>593</v>
+      </c>
+      <c r="C70">
+        <v>678</v>
+      </c>
+      <c r="D70">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>89</v>
+      </c>
+      <c r="B71">
+        <v>593</v>
+      </c>
+      <c r="C71">
+        <v>679</v>
+      </c>
+      <c r="D71">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>80</v>
+      </c>
+      <c r="B72">
+        <v>595</v>
+      </c>
+      <c r="C72">
+        <v>678</v>
+      </c>
+      <c r="D72">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>81</v>
+      </c>
+      <c r="B73">
+        <v>595</v>
+      </c>
+      <c r="C73">
+        <v>678</v>
+      </c>
+      <c r="D73">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>80</v>
+      </c>
+      <c r="B74">
+        <v>594</v>
+      </c>
+      <c r="C74">
+        <v>678</v>
+      </c>
+      <c r="D74">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>80</v>
+      </c>
+      <c r="B75">
+        <v>595</v>
+      </c>
+      <c r="C75">
+        <v>679</v>
+      </c>
+      <c r="D75">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>80</v>
+      </c>
+      <c r="B76">
+        <v>595</v>
+      </c>
+      <c r="C76">
+        <v>679</v>
+      </c>
+      <c r="D76">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>80</v>
+      </c>
+      <c r="B77">
+        <v>593</v>
+      </c>
+      <c r="C77">
+        <v>679</v>
+      </c>
+      <c r="D77">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>80</v>
+      </c>
+      <c r="B78">
+        <v>594</v>
+      </c>
+      <c r="C78">
+        <v>678</v>
+      </c>
+      <c r="D78">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>80</v>
+      </c>
+      <c r="B79">
+        <v>594</v>
+      </c>
+      <c r="C79">
+        <v>677</v>
+      </c>
+      <c r="D79">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>83</v>
+      </c>
+      <c r="B80">
+        <v>595</v>
+      </c>
+      <c r="C80">
+        <v>679</v>
+      </c>
+      <c r="D80">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>81</v>
+      </c>
+      <c r="B81">
+        <v>594</v>
+      </c>
+      <c r="C81">
+        <v>679</v>
+      </c>
+      <c r="D81">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <v>594</v>
+      </c>
+      <c r="C82">
+        <v>679</v>
+      </c>
+      <c r="D82">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>81</v>
+      </c>
+      <c r="B83">
+        <v>593</v>
+      </c>
+      <c r="C83">
+        <v>679</v>
+      </c>
+      <c r="D83">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>90</v>
+      </c>
+      <c r="B84">
+        <v>594</v>
+      </c>
+      <c r="C84">
+        <v>678</v>
+      </c>
+      <c r="D84">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>80</v>
+      </c>
+      <c r="B85">
+        <v>594</v>
+      </c>
+      <c r="C85">
+        <v>676</v>
+      </c>
+      <c r="D85">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>80</v>
+      </c>
+      <c r="B86">
+        <v>595</v>
+      </c>
+      <c r="C86">
+        <v>678</v>
+      </c>
+      <c r="D86">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>80</v>
+      </c>
+      <c r="B87">
+        <v>595</v>
+      </c>
+      <c r="C87">
+        <v>679</v>
+      </c>
+      <c r="D87">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>80</v>
+      </c>
+      <c r="B88">
+        <v>594</v>
+      </c>
+      <c r="C88">
+        <v>678</v>
+      </c>
+      <c r="D88">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>80</v>
+      </c>
+      <c r="B89">
+        <v>595</v>
+      </c>
+      <c r="C89">
+        <v>679</v>
+      </c>
+      <c r="D89">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>80</v>
+      </c>
+      <c r="B90">
+        <v>595</v>
+      </c>
+      <c r="C90">
+        <v>679</v>
+      </c>
+      <c r="D90">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>80</v>
+      </c>
+      <c r="B91">
+        <v>595</v>
+      </c>
+      <c r="C91">
+        <v>671</v>
+      </c>
+      <c r="D91">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>80</v>
+      </c>
+      <c r="B92">
+        <v>595</v>
+      </c>
+      <c r="C92">
+        <v>678</v>
+      </c>
+      <c r="D92">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>80</v>
+      </c>
+      <c r="B93">
+        <v>595</v>
+      </c>
+      <c r="C93">
+        <v>677</v>
+      </c>
+      <c r="D93">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>82</v>
+      </c>
+      <c r="B94">
+        <v>592</v>
+      </c>
+      <c r="C94">
+        <v>670</v>
+      </c>
+      <c r="D94">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>83</v>
+      </c>
+      <c r="B95">
+        <v>594</v>
+      </c>
+      <c r="C95">
+        <v>676</v>
+      </c>
+      <c r="D95">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>80</v>
+      </c>
+      <c r="B96">
+        <v>595</v>
+      </c>
+      <c r="C96">
+        <v>677</v>
+      </c>
+      <c r="D96">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>81</v>
+      </c>
+      <c r="B97">
+        <v>594</v>
+      </c>
+      <c r="C97">
+        <v>676</v>
+      </c>
+      <c r="D97">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>80</v>
+      </c>
+      <c r="B98">
+        <v>594</v>
+      </c>
+      <c r="C98">
+        <v>675</v>
+      </c>
+      <c r="D98">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>80</v>
+      </c>
+      <c r="B99">
+        <v>594</v>
+      </c>
+      <c r="C99">
+        <v>676</v>
+      </c>
+      <c r="D99">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>81</v>
+      </c>
+      <c r="B100">
+        <v>593</v>
+      </c>
+      <c r="C100">
+        <v>677</v>
+      </c>
+      <c r="D100">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>79</v>
+      </c>
+      <c r="B101">
+        <v>595</v>
+      </c>
+      <c r="C101">
+        <v>670</v>
+      </c>
+      <c r="D101">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>80</v>
+      </c>
+      <c r="B102">
+        <v>596</v>
+      </c>
+      <c r="C102">
+        <v>677</v>
+      </c>
+      <c r="D102">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>81</v>
+      </c>
+      <c r="B103">
+        <v>595</v>
+      </c>
+      <c r="C103">
+        <v>677</v>
+      </c>
+      <c r="D103">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>80</v>
+      </c>
+      <c r="B104">
+        <v>595</v>
+      </c>
+      <c r="C104">
+        <v>677</v>
+      </c>
+      <c r="D104">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>80</v>
+      </c>
+      <c r="B105">
+        <v>592</v>
+      </c>
+      <c r="C105">
+        <v>678</v>
+      </c>
+      <c r="D105">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>80</v>
+      </c>
+      <c r="B106">
+        <v>595</v>
+      </c>
+      <c r="C106">
+        <v>676</v>
+      </c>
+      <c r="D106">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>80</v>
+      </c>
+      <c r="B107">
+        <v>594</v>
+      </c>
+      <c r="C107">
+        <v>677</v>
+      </c>
+      <c r="D107">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>80</v>
+      </c>
+      <c r="B108">
+        <v>596</v>
+      </c>
+      <c r="C108">
+        <v>676</v>
+      </c>
+      <c r="D108">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>80</v>
+      </c>
+      <c r="B109">
+        <v>591</v>
+      </c>
+      <c r="C109">
+        <v>670</v>
+      </c>
+      <c r="D109">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>80</v>
+      </c>
+      <c r="B110">
+        <v>595</v>
+      </c>
+      <c r="C110">
+        <v>678</v>
+      </c>
+      <c r="D110">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>90</v>
+      </c>
+      <c r="B111">
+        <v>595</v>
+      </c>
+      <c r="C111">
+        <v>676</v>
+      </c>
+      <c r="D111">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>81</v>
+      </c>
+      <c r="B112">
+        <v>595</v>
+      </c>
+      <c r="C112">
+        <v>677</v>
+      </c>
+      <c r="D112">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>81</v>
+      </c>
+      <c r="B113">
+        <v>594</v>
+      </c>
+      <c r="C113">
+        <v>678</v>
+      </c>
+      <c r="D113">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>79</v>
+      </c>
+      <c r="B114">
+        <v>593</v>
+      </c>
+      <c r="C114">
+        <v>678</v>
+      </c>
+      <c r="D114">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>80</v>
+      </c>
+      <c r="B115">
+        <v>593</v>
+      </c>
+      <c r="C115">
+        <v>678</v>
+      </c>
+      <c r="D115">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>80</v>
+      </c>
+      <c r="B116">
+        <v>593</v>
+      </c>
+      <c r="C116">
+        <v>677</v>
+      </c>
+      <c r="D116">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>80</v>
+      </c>
+      <c r="B117">
+        <v>593</v>
+      </c>
+      <c r="C117">
+        <v>677</v>
+      </c>
+      <c r="D117">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>84</v>
+      </c>
+      <c r="B118">
+        <v>593</v>
+      </c>
+      <c r="D118">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>80</v>
+      </c>
+      <c r="B119">
+        <v>592</v>
+      </c>
+      <c r="D119">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>81</v>
+      </c>
+      <c r="B120">
+        <v>592</v>
+      </c>
+      <c r="D120">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>80</v>
+      </c>
+      <c r="B121">
+        <v>592</v>
+      </c>
+      <c r="D121">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>81</v>
+      </c>
+      <c r="B122">
+        <v>593</v>
+      </c>
+      <c r="D122">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>80</v>
+      </c>
+      <c r="B123">
+        <v>592</v>
+      </c>
+      <c r="D123">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>90</v>
+      </c>
+      <c r="B124">
+        <v>594</v>
+      </c>
+      <c r="D124">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>84</v>
+      </c>
+      <c r="B125">
+        <v>593</v>
+      </c>
+      <c r="D125">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <v>80</v>
+      </c>
+      <c r="B126">
+        <v>593</v>
+      </c>
+      <c r="D126">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>80</v>
+      </c>
+      <c r="B127">
+        <v>593</v>
+      </c>
+      <c r="D127">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>81</v>
+      </c>
+      <c r="B128">
+        <v>594</v>
+      </c>
+      <c r="D128">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>81</v>
+      </c>
+      <c r="B129">
+        <v>593</v>
+      </c>
+      <c r="D129">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <v>79</v>
+      </c>
+      <c r="B130">
+        <v>595</v>
+      </c>
+      <c r="D130">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <v>80</v>
+      </c>
+      <c r="B131">
+        <v>595</v>
+      </c>
+      <c r="D131">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A132">
+        <v>80</v>
+      </c>
+      <c r="B132">
+        <v>595</v>
+      </c>
+      <c r="D132">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A133">
+        <v>80</v>
+      </c>
+      <c r="B133">
+        <v>595</v>
+      </c>
+      <c r="D133">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B134">
+        <v>593</v>
+      </c>
+      <c r="D134">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B135">
+        <v>594</v>
+      </c>
+      <c r="D135">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B136">
+        <v>587</v>
+      </c>
+      <c r="D136">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B137">
+        <v>594</v>
+      </c>
+      <c r="D137">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B138">
+        <v>594</v>
+      </c>
+      <c r="D138">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B139">
+        <v>593</v>
+      </c>
+      <c r="D139">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B140">
+        <v>595</v>
+      </c>
+      <c r="D140">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B141">
+        <v>595</v>
+      </c>
+      <c r="D141">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B142">
+        <v>594</v>
+      </c>
+      <c r="D142">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B143">
+        <v>594</v>
+      </c>
+      <c r="D143">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B144">
+        <v>595</v>
+      </c>
+      <c r="D144">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="145" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B145">
+        <v>595</v>
+      </c>
+      <c r="D145">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="146" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B146">
+        <v>595</v>
+      </c>
+      <c r="D146">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="147" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B147">
+        <v>595</v>
+      </c>
+      <c r="D147">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="148" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B148">
+        <v>594</v>
+      </c>
+      <c r="D148">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="149" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B149">
+        <v>595</v>
+      </c>
+      <c r="D149">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="150" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B150">
+        <v>593</v>
+      </c>
+      <c r="D150">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="151" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B151">
+        <v>595</v>
+      </c>
+      <c r="D151">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="152" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B152">
+        <v>595</v>
+      </c>
+      <c r="D152">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="153" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B153">
+        <v>595</v>
+      </c>
+      <c r="D153">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="154" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B154">
+        <v>594</v>
+      </c>
+      <c r="D154">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="155" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B155">
+        <v>595</v>
+      </c>
+      <c r="D155">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="156" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B156">
+        <v>595</v>
+      </c>
+      <c r="D156">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="157" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B157">
+        <v>593</v>
+      </c>
+      <c r="D157">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="158" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B158">
+        <v>592</v>
+      </c>
+      <c r="D158">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="159" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B159">
+        <v>595</v>
+      </c>
+      <c r="D159">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="160" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B160">
+        <v>591</v>
+      </c>
+      <c r="D160">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="161" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B161">
+        <v>595</v>
+      </c>
+      <c r="D161">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="162" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B162">
+        <v>594</v>
+      </c>
+      <c r="D162">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="163" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B163">
+        <v>594</v>
+      </c>
+      <c r="D163">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="164" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B164">
+        <v>596</v>
+      </c>
+      <c r="D164">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="165" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B165">
+        <v>594</v>
+      </c>
+      <c r="D165">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="166" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B166">
+        <v>595</v>
+      </c>
+      <c r="D166">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="167" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B167">
+        <v>594</v>
+      </c>
+      <c r="D167">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="168" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B168">
+        <v>594</v>
+      </c>
+      <c r="D168">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="169" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B169">
+        <v>596</v>
+      </c>
+      <c r="D169">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="170" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B170">
+        <v>595</v>
+      </c>
+      <c r="D170">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="171" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B171">
+        <v>596</v>
+      </c>
+      <c r="D171">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="172" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B172">
+        <v>595</v>
+      </c>
+      <c r="D172">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="173" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B173">
+        <v>595</v>
+      </c>
+      <c r="D173">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="174" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B174">
+        <v>595</v>
+      </c>
+      <c r="D174">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="175" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B175">
+        <v>596</v>
+      </c>
+      <c r="D175">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="176" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B176">
+        <v>596</v>
+      </c>
+      <c r="D176">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="177" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B177">
+        <v>597</v>
+      </c>
+      <c r="D177">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="178" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B178">
+        <v>596</v>
+      </c>
+      <c r="D178">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="179" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B179">
+        <v>597</v>
+      </c>
+      <c r="D179">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="180" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B180">
+        <v>597</v>
+      </c>
+      <c r="D180">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="181" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B181">
+        <v>597</v>
+      </c>
+      <c r="D181">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="182" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B182">
+        <v>596</v>
+      </c>
+      <c r="D182">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="183" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B183">
+        <v>596</v>
+      </c>
+      <c r="D183">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="184" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B184">
+        <v>596</v>
+      </c>
+      <c r="D184">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="185" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B185">
+        <v>596</v>
+      </c>
+      <c r="D185">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="186" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B186">
+        <v>596</v>
+      </c>
+      <c r="D186">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="187" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B187">
+        <v>597</v>
+      </c>
+      <c r="D187">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="188" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B188">
+        <v>596</v>
+      </c>
+      <c r="D188">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="189" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B189">
+        <v>596</v>
+      </c>
+      <c r="D189">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="190" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B190">
+        <v>596</v>
+      </c>
+      <c r="D190">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="191" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B191">
+        <v>597</v>
+      </c>
+      <c r="D191">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="192" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B192">
+        <v>596</v>
+      </c>
+      <c r="D192">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="193" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B193">
+        <v>597</v>
+      </c>
+      <c r="D193">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="194" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B194">
+        <v>597</v>
+      </c>
+      <c r="D194">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="195" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B195">
+        <v>597</v>
+      </c>
+      <c r="D195">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="196" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B196">
+        <v>597</v>
+      </c>
+      <c r="D196">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="197" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B197">
+        <v>597</v>
+      </c>
+      <c r="D197">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="198" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B198">
+        <v>596</v>
+      </c>
+      <c r="D198">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="199" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B199">
+        <v>596</v>
+      </c>
+      <c r="D199">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="200" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B200">
+        <v>597</v>
+      </c>
+      <c r="D200">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="201" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B201">
+        <v>596</v>
+      </c>
+      <c r="D201">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="202" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B202">
+        <v>597</v>
+      </c>
+      <c r="D202">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="203" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B203">
+        <v>597</v>
+      </c>
+      <c r="D203">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="204" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B204">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="205" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B205">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="206" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B206">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="207" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B207">
+        <v>596</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>